<commit_message>
apontamentos - ajustes - V1
</commit_message>
<xml_diff>
--- a/backend/data/projects.xlsx
+++ b/backend/data/projects.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -407,15 +407,9 @@
         <v>Recid</v>
       </c>
       <c r="B1" t="str">
-        <v>mainContact</v>
+        <v>projId</v>
       </c>
       <c r="C1" t="str">
-        <v>companyId</v>
-      </c>
-      <c r="D1" t="str">
-        <v>projId</v>
-      </c>
-      <c r="E1" t="str">
         <v>refCompany</v>
       </c>
     </row>
@@ -424,21 +418,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v/>
+        <v>suporte Empresa 1</v>
       </c>
       <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v>projeto teste</v>
-      </c>
-      <c r="E2" t="str">
         <v>empresa teste 1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>